<commit_message>
Update to latest ASGS correspondences
</commit_message>
<xml_diff>
--- a/data-raw/asgs2016_2016gridcorrespondences/CG_SLA_2006_SA4_2016.xlsx
+++ b/data-raw/asgs2016_2016gridcorrespondences/CG_SLA_2006_SA4_2016.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Work\DATA.GOV update\Existing Data.gov files to be replaced\S_REFERENCE_ASGS_2016\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="165" windowWidth="15705" windowHeight="10575"/>
+    <workbookView xWindow="-90" yWindow="165" windowWidth="15705" windowHeight="10575" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="7" r:id="rId1"/>
@@ -30,7 +35,7 @@
     <definedName name="table1" localSheetId="5">Contents!#REF!</definedName>
     <definedName name="table1">Contents!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
   <webPublishing codePage="1252"/>
 </workbook>
 </file>
@@ -4768,7 +4773,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="57">
     <font>
       <sz val="8"/>
@@ -5908,6 +5913,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -5940,7 +5948,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -5948,6 +5956,16 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -6054,7 +6072,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -6062,6 +6080,16 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -6241,7 +6269,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -6249,6 +6277,16 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -6350,7 +6388,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -6358,6 +6396,16 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -6396,7 +6444,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -6404,6 +6452,16 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -6510,7 +6568,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -6518,6 +6576,16 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -6624,7 +6692,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -6632,6 +6700,16 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -6763,7 +6841,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6798,7 +6876,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7012,7 +7090,7 @@
   </sheetPr>
   <dimension ref="A1:N80"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
@@ -7368,7 +7446,7 @@
   <oleObjects>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Notes.Link" link="[1]!'!C58C0E00D46F25CA000000000000000000000000000000000000000000000000000000000000000000001D000000506572736F6E616C20576562204E6176696761746F72202852352E3029'" oleUpdate="OLEUPDATE_ALWAYS" shapeId="5121">
+        <oleObject link="[1]!'!C58C0E00D46F25CA000000000000000000000000000000000000000000000000000000000000000000001D000000506572736F6E616C20576562204E6176696761746F72202852352E3029'" oleUpdate="OLEUPDATE_ALWAYS" shapeId="5121">
           <objectPr defaultSize="0" autoPict="0" dde="1">
             <anchor moveWithCells="1">
               <from>
@@ -7388,7 +7466,7 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Notes.Link" link="[1]!'!C58C0E00D46F25CA000000000000000000000000000000000000000000000000000000000000000000001D000000506572736F6E616C20576562204E6176696761746F72202852352E3029'" oleUpdate="OLEUPDATE_ALWAYS" shapeId="5121"/>
+        <oleObject link="[1]!'!C58C0E00D46F25CA000000000000000000000000000000000000000000000000000000000000000000001D000000506572736F6E616C20576562204E6176696761746F72202852352E3029'" oleUpdate="OLEUPDATE_ALWAYS" shapeId="5121"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </oleObjects>
@@ -8182,7 +8260,7 @@
   <oleObjects>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Notes.Link" link="[1]!'!C58C0E00D46F25CA000000000000000000000000000000000000000000000000000000000000000000001D000000506572736F6E616C20576562204E6176696761746F72202852352E3029'" oleUpdate="OLEUPDATE_ALWAYS" shapeId="6145">
+        <oleObject link="[1]!'!C58C0E00D46F25CA000000000000000000000000000000000000000000000000000000000000000000001D000000506572736F6E616C20576562204E6176696761746F72202852352E3029'" oleUpdate="OLEUPDATE_ALWAYS" shapeId="6145">
           <objectPr defaultSize="0" autoPict="0" dde="1">
             <anchor moveWithCells="1">
               <from>
@@ -8202,7 +8280,7 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Notes.Link" link="[1]!'!C58C0E00D46F25CA000000000000000000000000000000000000000000000000000000000000000000001D000000506572736F6E616C20576562204E6176696761746F72202852352E3029'" oleUpdate="OLEUPDATE_ALWAYS" shapeId="6145"/>
+        <oleObject link="[1]!'!C58C0E00D46F25CA000000000000000000000000000000000000000000000000000000000000000000001D000000506572736F6E616C20576562204E6176696761746F72202852352E3029'" oleUpdate="OLEUPDATE_ALWAYS" shapeId="6145"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </oleObjects>
@@ -60229,7 +60307,7 @@
   <oleObjects>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Notes.Link" link="[1]!'!C58C0E00D46F25CA000000000000000000000000000000000000000000000000000000000000000000001D000000506572736F6E616C20576562204E6176696761746F72202852352E3029'" oleUpdate="OLEUPDATE_ALWAYS" shapeId="23553">
+        <oleObject link="[1]!'!C58C0E00D46F25CA000000000000000000000000000000000000000000000000000000000000000000001D000000506572736F6E616C20576562204E6176696761746F72202852352E3029'" oleUpdate="OLEUPDATE_ALWAYS" shapeId="23553">
           <objectPr defaultSize="0" autoPict="0" dde="1">
             <anchor moveWithCells="1">
               <from>
@@ -60249,12 +60327,12 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Notes.Link" link="[1]!'!C58C0E00D46F25CA000000000000000000000000000000000000000000000000000000000000000000001D000000506572736F6E616C20576562204E6176696761746F72202852352E3029'" oleUpdate="OLEUPDATE_ALWAYS" shapeId="23553"/>
+        <oleObject link="[1]!'!C58C0E00D46F25CA000000000000000000000000000000000000000000000000000000000000000000001D000000506572736F6E616C20576562204E6176696761746F72202852352E3029'" oleUpdate="OLEUPDATE_ALWAYS" shapeId="23553"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Notes.Link" link="[1]!'!C58C0E00D46F25CA000000000000000000000000000000000000000000000000000000000000000000001D000000506572736F6E616C20576562204E6176696761746F72202852352E3029'" oleUpdate="OLEUPDATE_ALWAYS" shapeId="23579">
+        <oleObject link="[1]!'!C58C0E00D46F25CA000000000000000000000000000000000000000000000000000000000000000000001D000000506572736F6E616C20576562204E6176696761746F72202852352E3029'" oleUpdate="OLEUPDATE_ALWAYS" shapeId="23579">
           <objectPr defaultSize="0" autoPict="0" dde="1">
             <anchor moveWithCells="1">
               <from>
@@ -60274,7 +60352,7 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Notes.Link" link="[1]!'!C58C0E00D46F25CA000000000000000000000000000000000000000000000000000000000000000000001D000000506572736F6E616C20576562204E6176696761746F72202852352E3029'" oleUpdate="OLEUPDATE_ALWAYS" shapeId="23579"/>
+        <oleObject link="[1]!'!C58C0E00D46F25CA000000000000000000000000000000000000000000000000000000000000000000001D000000506572736F6E616C20576562204E6176696761746F72202852352E3029'" oleUpdate="OLEUPDATE_ALWAYS" shapeId="23579"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </oleObjects>
@@ -61280,7 +61358,7 @@
   <oleObjects>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Notes.Link" link="[1]!'!C58C0E00D46F25CA000000000000000000000000000000000000000000000000000000000000000000001D000000506572736F6E616C20576562204E6176696761746F72202852352E3029'" oleUpdate="OLEUPDATE_ALWAYS" shapeId="24577">
+        <oleObject link="[1]!'!C58C0E00D46F25CA000000000000000000000000000000000000000000000000000000000000000000001D000000506572736F6E616C20576562204E6176696761746F72202852352E3029'" oleUpdate="OLEUPDATE_ALWAYS" shapeId="24577">
           <objectPr defaultSize="0" autoPict="0" dde="1">
             <anchor moveWithCells="1">
               <from>
@@ -61300,7 +61378,7 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Notes.Link" link="[1]!'!C58C0E00D46F25CA000000000000000000000000000000000000000000000000000000000000000000001D000000506572736F6E616C20576562204E6176696761746F72202852352E3029'" oleUpdate="OLEUPDATE_ALWAYS" shapeId="24577"/>
+        <oleObject link="[1]!'!C58C0E00D46F25CA000000000000000000000000000000000000000000000000000000000000000000001D000000506572736F6E616C20576562204E6176696761746F72202852352E3029'" oleUpdate="OLEUPDATE_ALWAYS" shapeId="24577"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </oleObjects>
@@ -64275,7 +64353,7 @@
   <oleObjects>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Notes.Link" link="[1]!'!C58C0E00D46F25CA000000000000000000000000000000000000000000000000000000000000000000001D000000506572736F6E616C20576562204E6176696761746F72202852352E3029'" oleUpdate="OLEUPDATE_ALWAYS" shapeId="25601">
+        <oleObject link="[1]!'!C58C0E00D46F25CA000000000000000000000000000000000000000000000000000000000000000000001D000000506572736F6E616C20576562204E6176696761746F72202852352E3029'" oleUpdate="OLEUPDATE_ALWAYS" shapeId="25601">
           <objectPr defaultSize="0" autoPict="0" dde="1">
             <anchor moveWithCells="1">
               <from>
@@ -64295,7 +64373,7 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Notes.Link" link="[1]!'!C58C0E00D46F25CA000000000000000000000000000000000000000000000000000000000000000000001D000000506572736F6E616C20576562204E6176696761746F72202852352E3029'" oleUpdate="OLEUPDATE_ALWAYS" shapeId="25601"/>
+        <oleObject link="[1]!'!C58C0E00D46F25CA000000000000000000000000000000000000000000000000000000000000000000001D000000506572736F6E616C20576562204E6176696761746F72202852352E3029'" oleUpdate="OLEUPDATE_ALWAYS" shapeId="25601"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </oleObjects>
@@ -66980,9 +67058,9 @@
   </sheetPr>
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -67225,7 +67303,7 @@
   <oleObjects>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Notes.Link" link="[1]!'!C58C0E00D46F25CA000000000000000000000000000000000000000000000000000000000000000000001D000000506572736F6E616C20576562204E6176696761746F72202852352E3029'" oleUpdate="OLEUPDATE_ALWAYS" shapeId="8193">
+        <oleObject link="[1]!'!C58C0E00D46F25CA000000000000000000000000000000000000000000000000000000000000000000001D000000506572736F6E616C20576562204E6176696761746F72202852352E3029'" oleUpdate="OLEUPDATE_ALWAYS" shapeId="8193">
           <objectPr defaultSize="0" autoPict="0" dde="1">
             <anchor moveWithCells="1">
               <from>
@@ -67245,7 +67323,7 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Notes.Link" link="[1]!'!C58C0E00D46F25CA000000000000000000000000000000000000000000000000000000000000000000001D000000506572736F6E616C20576562204E6176696761746F72202852352E3029'" oleUpdate="OLEUPDATE_ALWAYS" shapeId="8193"/>
+        <oleObject link="[1]!'!C58C0E00D46F25CA000000000000000000000000000000000000000000000000000000000000000000001D000000506572736F6E616C20576562204E6176696761746F72202852352E3029'" oleUpdate="OLEUPDATE_ALWAYS" shapeId="8193"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </oleObjects>

</xml_diff>